<commit_message>
primer commit sistema de legalizacion
</commit_message>
<xml_diff>
--- a/Factura_Ejemplo.xlsx
+++ b/Factura_Ejemplo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brangel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laragon\www\Laravel\accounting_flow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA556A-F504-4638-8B68-24F933EF2A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8CE5C9-0A7E-4B44-BD82-81F06E3D56AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="525" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Headers" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
   <si>
     <t>INVOICE_NUMBER</t>
   </si>
@@ -195,13 +195,13 @@
     <t>Lote-03</t>
   </si>
   <si>
-    <t>2025-0106</t>
-  </si>
-  <si>
-    <t>2025-0107</t>
-  </si>
-  <si>
-    <t>2025-0108</t>
+    <t>2025-0109</t>
+  </si>
+  <si>
+    <t>2025-0110</t>
+  </si>
+  <si>
+    <t>2025-0111</t>
   </si>
 </sst>
 </file>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -662,14 +662,14 @@
       <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
       </c>
       <c r="E2" s="3">
         <v>45672</v>
@@ -730,14 +730,14 @@
       <c r="A3" t="s">
         <v>54</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
       </c>
       <c r="E3" s="3">
         <v>45672</v>
@@ -798,14 +798,14 @@
       <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
       </c>
       <c r="E4" s="3">
         <v>45672</v>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>